<commit_message>
add file Signed-off-by: x30034819 <xieyijun3@huawei.com>
Signed-off-by: x30034819 <xieyijun3@huawei.com>
</commit_message>
<xml_diff>
--- a/rosen/modules/2d_graphics/test/适配问题_解决方式_汇总.xlsx
+++ b/rosen/modules/2d_graphics/test/适配问题_解决方式_汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24048" windowHeight="12420"/>
+    <workbookView windowWidth="29868" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+  <si>
+    <t>重点</t>
+  </si>
+  <si>
+    <t>用例适配原则：
+ 0、适配前先review一遍用例，看是否有缺失接口
+ 1、缺失的接口最好直接更换用例
+ 2、对外新增开放c接口，在写用例过程中基本不考虑
+ 3、如果是已经写的，写一半的代码，实在实现不了，直接放弃。但是代码上传，正常合入，做个标记
+ （a/用例处说明缺少哪些接口，b/用例不用全写完， c/在factory中汇总加一条说明，注释的形式）</t>
+  </si>
   <si>
     <t>序号</t>
   </si>
@@ -248,10 +259,18 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -763,139 +782,148 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -903,13 +931,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -979,13 +1007,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4930140</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>960120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1003,7 +1031,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="746760" y="1097280"/>
+          <a:off x="746760" y="2689860"/>
           <a:ext cx="4930140" cy="960120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1021,13 +1049,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2435225</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>695960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1045,92 +1073,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="746760" y="2062480"/>
+          <a:off x="746760" y="3655060"/>
           <a:ext cx="2435225" cy="695960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2302510</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>451485</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="图片 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="746760" y="3708400"/>
-          <a:ext cx="2302510" cy="451485"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2126615</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1059180</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="图片 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="746760" y="4805680"/>
-          <a:ext cx="2126615" cy="1059180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1152,27 +1096,27 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2659380</xdr:colOff>
+      <xdr:colOff>2302510</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>556260</xdr:rowOff>
+      <xdr:rowOff>451485</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="图片 4"/>
+        <xdr:cNvPr id="14" name="图片 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
+        <a:blip r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="746760" y="6558280"/>
-          <a:ext cx="2659380" cy="556260"/>
+          <a:off x="746760" y="5300980"/>
+          <a:ext cx="2302510" cy="451485"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1194,27 +1138,27 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2738120</xdr:colOff>
+      <xdr:colOff>2126615</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>700405</xdr:rowOff>
+      <xdr:rowOff>1059180</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="图片 5"/>
+        <xdr:cNvPr id="16" name="图片 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <a:blip r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="746760" y="7383780"/>
-          <a:ext cx="2738120" cy="700405"/>
+          <a:off x="746760" y="6398260"/>
+          <a:ext cx="2126615" cy="1059180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1236,27 +1180,27 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3267710</xdr:colOff>
+      <xdr:colOff>2659380</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>365760</xdr:rowOff>
+      <xdr:rowOff>556260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="图片 6"/>
+        <xdr:cNvPr id="18" name="图片 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <a:blip r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="746760" y="8221980"/>
-          <a:ext cx="3267710" cy="365760"/>
+          <a:off x="746760" y="8150860"/>
+          <a:ext cx="2659380" cy="556260"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1278,8 +1222,92 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
+      <xdr:colOff>2738120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>700405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="746760" y="8976360"/>
+          <a:ext cx="2738120" cy="700405"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3267710</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>365760</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="图片 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="746760" y="9814560"/>
+          <a:ext cx="3267710" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>2341880</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>249555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1297,7 +1325,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="746760" y="9867900"/>
+          <a:off x="746760" y="11460480"/>
           <a:ext cx="2341880" cy="249555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1311,13 +1339,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2333625</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>288925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1335,7 +1363,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="746760" y="10325100"/>
+          <a:off x="746760" y="11917680"/>
           <a:ext cx="2333625" cy="288925"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1349,13 +1377,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1516380</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1366,14 +1394,14 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11" r:link="rId12"/>
+        <a:blip r:embed="rId11" r:link="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9540240" y="10896600"/>
+          <a:off x="9540240" y="12489180"/>
           <a:ext cx="5204460" cy="1516380"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1640,10 +1668,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1654,169 +1682,181 @@
     <col min="5" max="5" width="44.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" ht="111" customHeight="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" ht="28.8" spans="1:5">
-      <c r="A2">
+    <row r="4" ht="28.8" spans="1:5">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" ht="43.2" spans="1:5">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="76" customHeight="1" spans="1:5">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="129.6" spans="1:5">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="86.4" spans="1:5">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" ht="138" customHeight="1" spans="1:5">
+      <c r="A9">
         <v>6</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" ht="43.2" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="10" ht="65" customHeight="1" spans="1:7">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" ht="66" customHeight="1" spans="1:5">
+      <c r="A11">
         <v>8</v>
       </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" ht="76" customHeight="1" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4"/>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
+    <row r="12" ht="129.6" spans="1:5">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" ht="129.6" spans="1:5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="13" ht="36" customHeight="1" spans="1:5">
+      <c r="A13">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" ht="45" customHeight="1" spans="1:5">
+      <c r="A14">
         <v>11</v>
       </c>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" ht="86.4" spans="1:5">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="15" ht="125" customHeight="1" spans="1:3">
+      <c r="A15">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" ht="138" customHeight="1" spans="1:5">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" ht="65" customHeight="1" spans="1:7">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" ht="66" customHeight="1" spans="1:5">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" ht="129.6" spans="1:5">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" ht="36" customHeight="1" spans="1:5">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" ht="45" customHeight="1" spans="1:5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" ht="125" customHeight="1" spans="1:3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>26</v>
+      <c r="B15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>